<commit_message>
datasource by entry and created new webpage
</commit_message>
<xml_diff>
--- a/Interview.Test2/DataSources/Data.xlsx
+++ b/Interview.Test2/DataSources/Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\New folder\Interview\Interview.Test2\DataSources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF56CAAC-AF66-402A-B8E0-1A158507B8F7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44436991-1B0B-4099-A8A5-79E796FBBAB5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{485695C9-2B4C-4F16-B26D-B7C8415B864D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="67">
   <si>
     <t>Email</t>
   </si>
@@ -66,13 +66,172 @@
     <t>Gov</t>
   </si>
   <si>
-    <t>a@gmail.com</t>
-  </si>
-  <si>
     <t>Aa1qwerty</t>
   </si>
   <si>
     <t>Initial</t>
+  </si>
+  <si>
+    <t>abs@gmail.com</t>
+  </si>
+  <si>
+    <t>plover@icloud.com</t>
+  </si>
+  <si>
+    <t>esasaki@icloud.com</t>
+  </si>
+  <si>
+    <t>jguyer@msn.com</t>
+  </si>
+  <si>
+    <t>dieman@live.com</t>
+  </si>
+  <si>
+    <t>penna@mac.com</t>
+  </si>
+  <si>
+    <t>lahvak@outlook.com</t>
+  </si>
+  <si>
+    <t>eabrown@sbcglobal.net</t>
+  </si>
+  <si>
+    <t>telbij@msn.com</t>
+  </si>
+  <si>
+    <t>yzheng@mac.com</t>
+  </si>
+  <si>
+    <t>benits@sbcglobal.net</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>GO</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>EP</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>Ingrid</t>
+  </si>
+  <si>
+    <t>Gogkiud</t>
+  </si>
+  <si>
+    <t>Orgrmo</t>
+  </si>
+  <si>
+    <t>Asgnlc</t>
+  </si>
+  <si>
+    <t>Megmam</t>
+  </si>
+  <si>
+    <t>Nogkook</t>
+  </si>
+  <si>
+    <t>Epgwnlobal</t>
+  </si>
+  <si>
+    <t>Atgjmo</t>
+  </si>
+  <si>
+    <t>Upggmo</t>
+  </si>
+  <si>
+    <t>Amgssobal</t>
+  </si>
+  <si>
+    <t>Nike</t>
+  </si>
+  <si>
+    <t>Oka</t>
+  </si>
+  <si>
+    <t>Rmke</t>
+  </si>
+  <si>
+    <t>Slka</t>
+  </si>
+  <si>
+    <t>Emaka</t>
+  </si>
+  <si>
+    <t>Ooka</t>
+  </si>
+  <si>
+    <t>Pko</t>
+  </si>
+  <si>
+    <t>Tmki</t>
+  </si>
+  <si>
+    <t>Pmkn</t>
+  </si>
+  <si>
+    <t>Mskt</t>
+  </si>
+  <si>
+    <t>pl@gmail.com</t>
+  </si>
+  <si>
+    <t>es@gomas.com</t>
+  </si>
+  <si>
+    <t>jg@gmamg.com</t>
+  </si>
+  <si>
+    <t>di@gmali.com</t>
+  </si>
+  <si>
+    <t>pe@gmamae.com</t>
+  </si>
+  <si>
+    <t>la@gomaoa.com</t>
+  </si>
+  <si>
+    <t>ea@gl.netaa.net</t>
+  </si>
+  <si>
+    <t>te@gmame.com</t>
+  </si>
+  <si>
+    <t>yz@gmamz.com</t>
+  </si>
+  <si>
+    <t>be@g.netase.net</t>
+  </si>
+  <si>
+    <t>Ss2Ghjahsfh</t>
+  </si>
+  <si>
+    <t>esS1sjfhasfh</t>
+  </si>
+  <si>
+    <t>Or1hshafhausf</t>
   </si>
 </sst>
 </file>
@@ -435,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B61DF12-164E-462F-A985-166789838CD9}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,13 +605,13 @@
     <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,7 +619,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -474,11 +633,8 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -495,20 +651,258 @@
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{3D4628AE-ADEC-4575-B6E4-9CE40D262B73}"/>
     <hyperlink ref="F2" r:id="rId2" xr:uid="{0EA36A4C-AE13-4DBD-AD4F-7EB11C00EA02}"/>
+    <hyperlink ref="F3" r:id="rId3" xr:uid="{E31FD63E-AA42-40DB-8B62-C84BC2757671}"/>
+    <hyperlink ref="F4" r:id="rId4" xr:uid="{BBC8E14A-B746-4F4C-A75B-C8521255E3A7}"/>
+    <hyperlink ref="F5" r:id="rId5" xr:uid="{D6EDE979-475A-4C4C-B20B-E870142EB989}"/>
+    <hyperlink ref="F6" r:id="rId6" xr:uid="{39D1FC05-DCF6-4168-9B9E-CA4CEADF5869}"/>
+    <hyperlink ref="F7" r:id="rId7" xr:uid="{EC35414F-2AAC-4603-9288-ACB3991C3A81}"/>
+    <hyperlink ref="F8" r:id="rId8" xr:uid="{44D8F176-AAAD-4DCF-BFCC-CFA5BBF829E3}"/>
+    <hyperlink ref="F9" r:id="rId9" xr:uid="{B6E570FA-E1B3-43BD-A824-276AB176B626}"/>
+    <hyperlink ref="F10" r:id="rId10" xr:uid="{84D4695B-A22E-4635-B00A-6709A4C38F1E}"/>
+    <hyperlink ref="F11" r:id="rId11" xr:uid="{5C1A152E-4CE1-4CCA-8336-9E284A978AB4}"/>
+    <hyperlink ref="F12" r:id="rId12" xr:uid="{AA7CB48E-2D6C-421A-836D-08423AE41FE7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>